<commit_message>
minor change in Data.xlsx
</commit_message>
<xml_diff>
--- a/Documentation/Data - 2012.xlsx
+++ b/Documentation/Data - 2012.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17766"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johan\Desktop\IBMDESC-Poverty\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mlbel\Desktop\IBMDESC-Poverty\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -180,9 +180,6 @@
     <t>7,913.56 sq mi</t>
   </si>
   <si>
-    <t>7,860.04 sq mi)</t>
-  </si>
-  <si>
     <t>8,692.43 sq mi</t>
   </si>
   <si>
@@ -332,6 +329,9 @@
   <si>
     <t>Poverty Incidence
 among population 2015(%)</t>
+  </si>
+  <si>
+    <t>7,860.04 sq mi</t>
   </si>
 </sst>
 </file>
@@ -759,8 +759,8 @@
   <dimension ref="A1:Q18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="M1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H2" sqref="H2"/>
+      <pane xSplit="1" topLeftCell="L1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -789,46 +789,46 @@
         <v>36</v>
       </c>
       <c r="D1" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="F1" s="9" t="s">
         <v>63</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>64</v>
       </c>
       <c r="G1" s="8" t="s">
         <v>37</v>
       </c>
       <c r="H1" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="K1" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="I1" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="J1" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="K1" s="9" t="s">
-        <v>73</v>
-      </c>
       <c r="L1" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="M1" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="M1" s="9" t="s">
+      <c r="N1" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="O1" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="N1" s="9" t="s">
+      <c r="P1" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="O1" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="P1" s="9" t="s">
+      <c r="Q1" s="9" t="s">
         <v>69</v>
-      </c>
-      <c r="Q1" s="9" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -1540,7 +1540,7 @@
         <v>1156</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>51</v>
+        <v>74</v>
       </c>
       <c r="H15" s="1">
         <v>30.7</v>
@@ -1593,7 +1593,7 @@
         <v>1055</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H16" s="1">
         <v>44.7</v>
@@ -1646,7 +1646,7 @@
         <v>579</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H17" s="1">
         <v>40.299999999999997</v>
@@ -1699,7 +1699,7 @@
         <v>616</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H18" s="1">
         <v>53.7</v>
@@ -1750,37 +1750,37 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>